<commit_message>
Fix most previous problem. To-do: redo all the MC/MR work
</commit_message>
<xml_diff>
--- a/document/temporal.xlsx
+++ b/document/temporal.xlsx
@@ -4,13 +4,17 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="walking" sheetId="1" r:id="rId1"/>
     <sheet name="weekday" sheetId="2" r:id="rId2"/>
     <sheet name="hour" sheetId="3" r:id="rId3"/>
+    <sheet name="ER_memory_and_function" sheetId="4" r:id="rId4"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>GR</t>
   </si>
@@ -88,18 +92,36 @@
   <si>
     <t>NR miss risk</t>
   </si>
+  <si>
+    <t>minimizing AWT</t>
+  </si>
+  <si>
+    <t>averaging AWT</t>
+  </si>
+  <si>
+    <t>minimizing WT deviation</t>
+  </si>
+  <si>
+    <t>averaging WT deviation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -122,8 +144,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -697,34 +720,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>189</c:v>
+                  <c:v>224</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>189</c:v>
+                  <c:v>224</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>189</c:v>
+                  <c:v>224</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>189</c:v>
+                  <c:v>224</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>189</c:v>
+                  <c:v>224</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>189</c:v>
+                  <c:v>224</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>189</c:v>
+                  <c:v>224</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>189</c:v>
+                  <c:v>224</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>189</c:v>
+                  <c:v>224</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>189</c:v>
+                  <c:v>224</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2297,25 +2320,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>158.94164363163301</c:v>
+                  <c:v>200.47720612480501</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>174.286737613231</c:v>
+                  <c:v>209.22960598729699</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>179.47536631352801</c:v>
+                  <c:v>211.72561107155099</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>192.767221241035</c:v>
+                  <c:v>222.066034979455</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>230.039046169568</c:v>
+                  <c:v>247.732925800723</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>159.48353187456999</c:v>
+                  <c:v>226.36104320700599</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>232.869887968862</c:v>
+                  <c:v>256.79484454481502</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2874,64 +2897,64 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21.870634128640098</c:v>
+                  <c:v>124.622747747747</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>133.77846974259501</c:v>
+                  <c:v>159.085292262504</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>150.59624914633901</c:v>
+                  <c:v>176.98252154143299</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>139.839867215699</c:v>
+                  <c:v>168.181430857382</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>165.84866394603799</c:v>
+                  <c:v>197.43502806570001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>173.42338624657299</c:v>
+                  <c:v>204.351572845802</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>175.71798684190199</c:v>
+                  <c:v>212.28838994567801</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>178.91654931353199</c:v>
+                  <c:v>216.76752421542</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>206.65673027776299</c:v>
+                  <c:v>244.13042630671899</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>207.795915456031</c:v>
+                  <c:v>247.81993904488101</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>197.18121402611999</c:v>
+                  <c:v>239.182780203318</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>195.17315672856799</c:v>
+                  <c:v>231.081816705329</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>202.39000263899899</c:v>
+                  <c:v>231.91511537801699</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>230.69250764758701</c:v>
+                  <c:v>255.052313529099</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>223.83907348077699</c:v>
+                  <c:v>249.101015373243</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>202.975968159324</c:v>
+                  <c:v>239.74285973961</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>183.639743788647</c:v>
+                  <c:v>227.91725383359301</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>221.171930597444</c:v>
+                  <c:v>260.80017270963401</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>214.709901134403</c:v>
+                  <c:v>252.588714474754</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>153.510070476999</c:v>
+                  <c:v>239.206935708321</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3849,6 +3872,576 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11592825896762905"/>
+          <c:y val="5.0925925925925923E-2"/>
+          <c:w val="0.85351618547681551"/>
+          <c:h val="0.78054024496937879"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ER_memory_and_function!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>minimizing AWT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ER_memory_and_function!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ER_memory_and_function!$B$2:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>430.32763429299098</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>367.858722476043</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>375.87304476912198</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>341.33818036837499</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>312.330035847342</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>290.77447844038699</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>320.52019937256199</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>314.66773568764103</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>311.90058835884702</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-D790-4E14-8607-478512457AAE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ER_memory_and_function!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>averaging AWT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ER_memory_and_function!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ER_memory_and_function!$D$2:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>430.52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>478.18174233321201</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>492.15089282967102</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>524.80041549351597</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>547.51</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>564.07000000000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>565.07000000000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>568.54999999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>570.69000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-D790-4E14-8607-478512457AAE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1543104767"/>
+        <c:axId val="1543105183"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1543104767"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Memory period</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.80666666666666664"/>
+              <c:y val="0.92497666958296876"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1543105183"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1543105183"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="250"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Waiting</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> time (seconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1543104767"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.2287823709536308"/>
+          <c:y val="0.90798556430446198"/>
+          <c:w val="0.5424352580927384"/>
+          <c:h val="7.8125546806649182E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4009,6 +4602,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -5519,6 +6152,522 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6167,6 +7316,134 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>average waiting time</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2">
+            <v>1</v>
+          </cell>
+          <cell r="B2">
+            <v>629.58000000000004</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>2</v>
+          </cell>
+          <cell r="B3">
+            <v>506.24</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>3</v>
+          </cell>
+          <cell r="B4">
+            <v>512.37</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>4</v>
+          </cell>
+          <cell r="B5">
+            <v>445.66</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>5</v>
+          </cell>
+          <cell r="B6">
+            <v>395.86</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>6</v>
+          </cell>
+          <cell r="B7">
+            <v>360.56</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>7</v>
+          </cell>
+          <cell r="B8">
+            <v>404.69</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>8</v>
+          </cell>
+          <cell r="B9">
+            <v>394.13</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>9</v>
+          </cell>
+          <cell r="B10">
+            <v>388.57</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6434,11 +7711,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1">
@@ -6612,39 +7892,39 @@
         <v>509</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>189</v>
-      </c>
-      <c r="C6">
-        <v>189</v>
-      </c>
-      <c r="D6">
-        <v>189</v>
-      </c>
-      <c r="E6">
-        <v>189</v>
-      </c>
-      <c r="F6">
-        <v>189</v>
-      </c>
-      <c r="G6">
-        <v>189</v>
-      </c>
-      <c r="H6">
-        <v>189</v>
-      </c>
-      <c r="I6">
-        <v>189</v>
-      </c>
-      <c r="J6">
-        <v>189</v>
-      </c>
-      <c r="K6">
-        <v>189</v>
+      <c r="B6" s="1">
+        <v>224</v>
+      </c>
+      <c r="C6" s="1">
+        <v>224</v>
+      </c>
+      <c r="D6" s="1">
+        <v>224</v>
+      </c>
+      <c r="E6" s="1">
+        <v>224</v>
+      </c>
+      <c r="F6" s="1">
+        <v>224</v>
+      </c>
+      <c r="G6" s="1">
+        <v>224</v>
+      </c>
+      <c r="H6" s="1">
+        <v>224</v>
+      </c>
+      <c r="I6" s="1">
+        <v>224</v>
+      </c>
+      <c r="J6" s="1">
+        <v>224</v>
+      </c>
+      <c r="K6" s="1">
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -6821,7 +8101,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6830,7 +8111,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6944,25 +8225,25 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>158.94164363163301</v>
+        <v>200.47720612480501</v>
       </c>
       <c r="C5">
-        <v>174.286737613231</v>
+        <v>209.22960598729699</v>
       </c>
       <c r="D5">
-        <v>179.47536631352801</v>
+        <v>211.72561107155099</v>
       </c>
       <c r="E5">
-        <v>192.767221241035</v>
+        <v>222.066034979455</v>
       </c>
       <c r="F5">
-        <v>230.039046169568</v>
+        <v>247.732925800723</v>
       </c>
       <c r="G5">
-        <v>159.48353187456999</v>
+        <v>226.36104320700599</v>
       </c>
       <c r="H5">
-        <v>232.869887968862</v>
+        <v>256.79484454481502</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -6999,7 +8280,7 @@
   <dimension ref="A1:Y8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7175,64 +8456,64 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>21.870634128640098</v>
+        <v>124.622747747747</v>
       </c>
       <c r="G3">
-        <v>133.77846974259501</v>
+        <v>159.085292262504</v>
       </c>
       <c r="H3">
-        <v>150.59624914633901</v>
+        <v>176.98252154143299</v>
       </c>
       <c r="I3">
-        <v>139.839867215699</v>
+        <v>168.181430857382</v>
       </c>
       <c r="J3">
-        <v>165.84866394603799</v>
+        <v>197.43502806570001</v>
       </c>
       <c r="K3">
-        <v>173.42338624657299</v>
+        <v>204.351572845802</v>
       </c>
       <c r="L3">
-        <v>175.71798684190199</v>
+        <v>212.28838994567801</v>
       </c>
       <c r="M3">
-        <v>178.91654931353199</v>
+        <v>216.76752421542</v>
       </c>
       <c r="N3">
-        <v>206.65673027776299</v>
+        <v>244.13042630671899</v>
       </c>
       <c r="O3">
-        <v>207.795915456031</v>
+        <v>247.81993904488101</v>
       </c>
       <c r="P3">
-        <v>197.18121402611999</v>
+        <v>239.182780203318</v>
       </c>
       <c r="Q3">
-        <v>195.17315672856799</v>
+        <v>231.081816705329</v>
       </c>
       <c r="R3">
-        <v>202.39000263899899</v>
+        <v>231.91511537801699</v>
       </c>
       <c r="S3">
-        <v>230.69250764758701</v>
+        <v>255.052313529099</v>
       </c>
       <c r="T3">
-        <v>223.83907348077699</v>
+        <v>249.101015373243</v>
       </c>
       <c r="U3">
-        <v>202.975968159324</v>
+        <v>239.74285973961</v>
       </c>
       <c r="V3">
-        <v>183.639743788647</v>
+        <v>227.91725383359301</v>
       </c>
       <c r="W3">
-        <v>221.171930597444</v>
+        <v>260.80017270963401</v>
       </c>
       <c r="X3">
-        <v>214.709901134403</v>
+        <v>252.588714474754</v>
       </c>
       <c r="Y3">
-        <v>153.510070476999</v>
+        <v>239.206935708321</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -7541,6 +8822,192 @@
       </c>
       <c r="Y8">
         <v>883748</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="5" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>430.32763429299098</v>
+      </c>
+      <c r="C2">
+        <v>570.04889499983506</v>
+      </c>
+      <c r="D2">
+        <v>430.52</v>
+      </c>
+      <c r="E2">
+        <v>570.21470750598803</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>367.858722476043</v>
+      </c>
+      <c r="C3">
+        <v>521.02586992160502</v>
+      </c>
+      <c r="D3">
+        <v>478.18174233321201</v>
+      </c>
+      <c r="E3">
+        <v>596.05471901603698</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>375.87304476912198</v>
+      </c>
+      <c r="C4">
+        <v>587.68501809953898</v>
+      </c>
+      <c r="D4">
+        <v>492.15089282967102</v>
+      </c>
+      <c r="E4">
+        <v>658.96212313946103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>341.33818036837499</v>
+      </c>
+      <c r="C5">
+        <v>542.25184048752396</v>
+      </c>
+      <c r="D5">
+        <v>524.80041549351597</v>
+      </c>
+      <c r="E5">
+        <v>678.147575806384</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>312.330035847342</v>
+      </c>
+      <c r="C6">
+        <v>507.74513375374698</v>
+      </c>
+      <c r="D6">
+        <v>547.51</v>
+      </c>
+      <c r="E6">
+        <v>696.36591030659895</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>290.77447844038699</v>
+      </c>
+      <c r="C7">
+        <v>479.68644949396099</v>
+      </c>
+      <c r="D7">
+        <v>564.07000000000005</v>
+      </c>
+      <c r="E7">
+        <v>703.67759550472897</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>320.52019937256199</v>
+      </c>
+      <c r="C8">
+        <v>495.56350409804702</v>
+      </c>
+      <c r="D8">
+        <v>565.07000000000005</v>
+      </c>
+      <c r="E8">
+        <v>693.89808395864395</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>314.66773568764103</v>
+      </c>
+      <c r="C9">
+        <v>486.98349376645399</v>
+      </c>
+      <c r="D9">
+        <v>568.54999999999995</v>
+      </c>
+      <c r="E9">
+        <v>694.49280109017798</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>311.90058835884702</v>
+      </c>
+      <c r="C10">
+        <v>482.46480953247499</v>
+      </c>
+      <c r="D10">
+        <v>570.69000000000005</v>
+      </c>
+      <c r="E10">
+        <v>695.37484435516001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the draft and fix almost all Missed rate calculation result.
</commit_message>
<xml_diff>
--- a/document/temporal.xlsx
+++ b/document/temporal.xlsx
@@ -12,9 +12,6 @@
     <sheet name="hour" sheetId="3" r:id="rId3"/>
     <sheet name="ER_memory_and_function" sheetId="4" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1186,34 +1183,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>12.354250022956386</c:v>
+                  <c:v>61.895099238493998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.79387334956637</c:v>
+                  <c:v>64.855108869195405</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.391610335899351</c:v>
+                  <c:v>64.56569456820435</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.93768609849716</c:v>
+                  <c:v>63.960593231504333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.494534208596875</c:v>
+                  <c:v>63.155326380440492</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.918555472632782</c:v>
+                  <c:v>62.220579348256223</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.259532230681888</c:v>
+                  <c:v>61.587561475131672</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.5853687088434771</c:v>
+                  <c:v>60.522799305501621</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.9677410889432689</c:v>
+                  <c:v>59.530757606572934</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.2873413651423107</c:v>
+                  <c:v>58.65542647664109</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1294,34 +1291,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.1965265064525501</c:v>
+                  <c:v>2.06353112128674</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.1963046139081599</c:v>
+                  <c:v>2.4918225452438403</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1174912547820099</c:v>
+                  <c:v>2.8153417648856101</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2580957154793699</c:v>
+                  <c:v>3.0881471354135801</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2091532121303397</c:v>
+                  <c:v>3.3579077141734199</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1488794674852101</c:v>
+                  <c:v>3.6367871630851201</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.1565831121105501</c:v>
+                  <c:v>3.9427732146170098</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.09008684881944</c:v>
+                  <c:v>4.2576385151629799</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.0429742948521201</c:v>
+                  <c:v>4.6237726900929204</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.9887504546775399</c:v>
+                  <c:v>5.01129407199425</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7355,97 +7352,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>average waiting time</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2">
-            <v>1</v>
-          </cell>
-          <cell r="B2">
-            <v>629.58000000000004</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3">
-            <v>2</v>
-          </cell>
-          <cell r="B3">
-            <v>506.24</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>3</v>
-          </cell>
-          <cell r="B4">
-            <v>512.37</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>4</v>
-          </cell>
-          <cell r="B5">
-            <v>445.66</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>5</v>
-          </cell>
-          <cell r="B6">
-            <v>395.86</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>6</v>
-          </cell>
-          <cell r="B7">
-            <v>360.56</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8">
-            <v>7</v>
-          </cell>
-          <cell r="B8">
-            <v>404.69</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9">
-            <v>8</v>
-          </cell>
-          <cell r="B9">
-            <v>394.13</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10">
-            <v>9</v>
-          </cell>
-          <cell r="B10">
-            <v>388.57</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7712,7 +7618,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7964,34 +7870,34 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>12.354250022956386</v>
+        <v>61.895099238493998</v>
       </c>
       <c r="C16">
-        <v>12.79387334956637</v>
+        <v>64.855108869195405</v>
       </c>
       <c r="D16">
-        <v>12.391610335899351</v>
+        <v>64.56569456820435</v>
       </c>
       <c r="E16">
-        <v>11.93768609849716</v>
+        <v>63.960593231504333</v>
       </c>
       <c r="F16">
-        <v>11.494534208596875</v>
+        <v>63.155326380440492</v>
       </c>
       <c r="G16">
-        <v>10.918555472632782</v>
+        <v>62.220579348256223</v>
       </c>
       <c r="H16">
-        <v>10.259532230681888</v>
+        <v>61.587561475131672</v>
       </c>
       <c r="I16">
-        <v>9.5853687088434771</v>
+        <v>60.522799305501621</v>
       </c>
       <c r="J16">
-        <v>8.9677410889432689</v>
+        <v>59.530757606572934</v>
       </c>
       <c r="K16">
-        <v>8.2873413651423107</v>
+        <v>58.65542647664109</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -7999,34 +7905,34 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>2.1965265064525501</v>
+        <v>2.06353112128674</v>
       </c>
       <c r="C17">
-        <v>2.1963046139081599</v>
+        <v>2.4918225452438403</v>
       </c>
       <c r="D17">
-        <v>2.1174912547820099</v>
+        <v>2.8153417648856101</v>
       </c>
       <c r="E17">
-        <v>2.2580957154793699</v>
+        <v>3.0881471354135801</v>
       </c>
       <c r="F17">
-        <v>2.2091532121303397</v>
+        <v>3.3579077141734199</v>
       </c>
       <c r="G17">
-        <v>2.1488794674852101</v>
+        <v>3.6367871630851201</v>
       </c>
       <c r="H17">
-        <v>2.1565831121105501</v>
+        <v>3.9427732146170098</v>
       </c>
       <c r="I17">
-        <v>2.09008684881944</v>
+        <v>4.2576385151629799</v>
       </c>
       <c r="J17">
-        <v>2.0429742948521201</v>
+        <v>4.6237726900929204</v>
       </c>
       <c r="K17">
-        <v>1.9887504546775399</v>
+        <v>5.01129407199425</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -8111,7 +8017,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8835,7 +8741,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update new PR optimal's contents in the draft
</commit_message>
<xml_diff>
--- a/document/temporal.xlsx
+++ b/document/temporal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="walking" sheetId="1" r:id="rId1"/>
@@ -370,34 +370,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>199.726396985294</c:v>
+                  <c:v>183.568265720976</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>206.49628215204399</c:v>
+                  <c:v>192.74554685722899</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>211.941271610934</c:v>
+                  <c:v>200.71206304120699</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>217.709047741419</c:v>
+                  <c:v>209.03298151981201</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>223.865850583314</c:v>
+                  <c:v>218.53204337750299</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>230.70529080970999</c:v>
+                  <c:v>228.94000613574801</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>237.644081567819</c:v>
+                  <c:v>240.104771669754</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>244.77049068151999</c:v>
+                  <c:v>250.42900767010499</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>251.45978937105099</c:v>
+                  <c:v>260.414828552296</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>258.08702297038502</c:v>
+                  <c:v>270.12133922757499</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1291,34 +1291,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.06353112128674</c:v>
+                  <c:v>4.85581424731601</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4918225452438403</c:v>
+                  <c:v>5.4754738818729294</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.8153417648856101</c:v>
+                  <c:v>6.11524316017577</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0881471354135801</c:v>
+                  <c:v>6.7943622108055104</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.3579077141734199</c:v>
+                  <c:v>7.6340429643105594</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.6367871630851201</c:v>
+                  <c:v>8.5547984204005196</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.9427732146170098</c:v>
+                  <c:v>9.5561641449912305</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.2576385151629799</c:v>
+                  <c:v>10.459176307273101</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.6237726900929204</c:v>
+                  <c:v>11.3813068616137</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.01129407199425</c:v>
+                  <c:v>12.2939874813058</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1416,34 +1416,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>14.89</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>14.89</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>14.89</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>14.89</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>14.89</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>14.89</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>14.89</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>14.89</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>14.89</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>14.89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1527,34 +1527,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3.8</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.8</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.8</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.8</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.8</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.8</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.8</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.8</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.8</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2228,25 +2228,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>239.659639179317</c:v>
+                  <c:v>219.564688103143</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>238.03576719595199</c:v>
+                  <c:v>217.223064698793</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>237.341429771208</c:v>
+                  <c:v>214.43330715886401</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>236.81810869930999</c:v>
+                  <c:v>213.515893044416</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>242.003065720531</c:v>
+                  <c:v>218.028200051543</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>198.56744064898399</c:v>
+                  <c:v>260.089103131223</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>192.31555533565901</c:v>
+                  <c:v>245.57931763887399</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2696,67 +2696,67 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>91.05</c:v>
+                  <c:v>118.15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>223.53044556120301</c:v>
+                  <c:v>201.97619828468601</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>222.24239920925399</c:v>
+                  <c:v>226.42648579435399</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>230.46947555136001</c:v>
+                  <c:v>230.60930894672899</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>225.17640490949901</c:v>
+                  <c:v>210.115538224071</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>224.16178352043701</c:v>
+                  <c:v>208.131678039924</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>215.196060324852</c:v>
+                  <c:v>214.53178251581801</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>216.340022897295</c:v>
+                  <c:v>218.09942244320601</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>221.77321159864201</c:v>
+                  <c:v>222.733836741636</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>224.53311342119301</c:v>
+                  <c:v>226.98496644718401</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>223.12048446370801</c:v>
+                  <c:v>224.11626102007301</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>232.480820727777</c:v>
+                  <c:v>224.164804497365</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>231.88552653420899</c:v>
+                  <c:v>211.17234330888201</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>233.96426681462501</c:v>
+                  <c:v>207.99419973303401</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>233.50808146155001</c:v>
+                  <c:v>213.45798580293399</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>223.27183658974201</c:v>
+                  <c:v>211.49503265162099</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>219.87444725693899</c:v>
+                  <c:v>221.388463865094</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>220.25200205761701</c:v>
+                  <c:v>235.225607808886</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>217.95717703185201</c:v>
+                  <c:v>239.971586446266</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>273.00522467454999</c:v>
+                  <c:v>340.37994583711099</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>347.13972308848201</c:v>
+                  <c:v>457.58083398530403</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7618,7 +7618,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7698,34 +7698,34 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>199.726396985294</v>
+        <v>183.568265720976</v>
       </c>
       <c r="C3">
-        <v>206.49628215204399</v>
+        <v>192.74554685722899</v>
       </c>
       <c r="D3">
-        <v>211.941271610934</v>
+        <v>200.71206304120699</v>
       </c>
       <c r="E3">
-        <v>217.709047741419</v>
+        <v>209.03298151981201</v>
       </c>
       <c r="F3">
-        <v>223.865850583314</v>
+        <v>218.53204337750299</v>
       </c>
       <c r="G3">
-        <v>230.70529080970999</v>
+        <v>228.94000613574801</v>
       </c>
       <c r="H3">
-        <v>237.644081567819</v>
+        <v>240.104771669754</v>
       </c>
       <c r="I3">
-        <v>244.77049068151999</v>
+        <v>250.42900767010499</v>
       </c>
       <c r="J3">
-        <v>251.45978937105099</v>
+        <v>260.414828552296</v>
       </c>
       <c r="K3">
-        <v>258.08702297038502</v>
+        <v>270.12133922757499</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -7905,34 +7905,34 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>2.06353112128674</v>
+        <v>4.85581424731601</v>
       </c>
       <c r="C17">
-        <v>2.4918225452438403</v>
+        <v>5.4754738818729294</v>
       </c>
       <c r="D17">
-        <v>2.8153417648856101</v>
+        <v>6.11524316017577</v>
       </c>
       <c r="E17">
-        <v>3.0881471354135801</v>
+        <v>6.7943622108055104</v>
       </c>
       <c r="F17">
-        <v>3.3579077141734199</v>
+        <v>7.6340429643105594</v>
       </c>
       <c r="G17">
-        <v>3.6367871630851201</v>
+        <v>8.5547984204005196</v>
       </c>
       <c r="H17">
-        <v>3.9427732146170098</v>
+        <v>9.5561641449912305</v>
       </c>
       <c r="I17">
-        <v>4.2576385151629799</v>
+        <v>10.459176307273101</v>
       </c>
       <c r="J17">
-        <v>4.6237726900929204</v>
+        <v>11.3813068616137</v>
       </c>
       <c r="K17">
-        <v>5.01129407199425</v>
+        <v>12.2939874813058</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -7940,34 +7940,34 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>14.89</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>14.89</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>14.89</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>14.89</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>14.89</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>14.89</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>14.89</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>14.89</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>14.89</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>14.89</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -7975,34 +7975,34 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
       <c r="C19">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
       <c r="D19">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
       <c r="E19">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
       <c r="F19">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
       <c r="G19">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
       <c r="H19">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
       <c r="I19">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
       <c r="J19">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
       <c r="K19">
-        <v>3.8</v>
+        <v>3.7</v>
       </c>
     </row>
   </sheetData>
@@ -8017,7 +8017,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8105,25 +8105,25 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>239.659639179317</v>
+        <v>219.564688103143</v>
       </c>
       <c r="C4">
-        <v>238.03576719595199</v>
+        <v>217.223064698793</v>
       </c>
       <c r="D4">
-        <v>237.341429771208</v>
+        <v>214.43330715886401</v>
       </c>
       <c r="E4">
-        <v>236.81810869930999</v>
+        <v>213.515893044416</v>
       </c>
       <c r="F4">
-        <v>242.003065720531</v>
+        <v>218.028200051543</v>
       </c>
       <c r="G4">
-        <v>198.56744064898399</v>
+        <v>260.089103131223</v>
       </c>
       <c r="H4">
-        <v>192.31555533565901</v>
+        <v>245.57931763887399</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -8185,8 +8185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8282,67 +8282,67 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>91.05</v>
+        <v>118.15</v>
       </c>
       <c r="F2">
-        <v>223.53044556120301</v>
+        <v>201.97619828468601</v>
       </c>
       <c r="G2">
-        <v>222.24239920925399</v>
+        <v>226.42648579435399</v>
       </c>
       <c r="H2">
-        <v>230.46947555136001</v>
+        <v>230.60930894672899</v>
       </c>
       <c r="I2">
-        <v>225.17640490949901</v>
+        <v>210.115538224071</v>
       </c>
       <c r="J2">
-        <v>224.16178352043701</v>
+        <v>208.131678039924</v>
       </c>
       <c r="K2">
-        <v>215.196060324852</v>
+        <v>214.53178251581801</v>
       </c>
       <c r="L2">
-        <v>216.340022897295</v>
+        <v>218.09942244320601</v>
       </c>
       <c r="M2">
-        <v>221.77321159864201</v>
+        <v>222.733836741636</v>
       </c>
       <c r="N2">
-        <v>224.53311342119301</v>
+        <v>226.98496644718401</v>
       </c>
       <c r="O2">
-        <v>223.12048446370801</v>
+        <v>224.11626102007301</v>
       </c>
       <c r="P2">
-        <v>232.480820727777</v>
+        <v>224.164804497365</v>
       </c>
       <c r="Q2">
-        <v>231.88552653420899</v>
+        <v>211.17234330888201</v>
       </c>
       <c r="R2">
-        <v>233.96426681462501</v>
+        <v>207.99419973303401</v>
       </c>
       <c r="S2">
-        <v>233.50808146155001</v>
+        <v>213.45798580293399</v>
       </c>
       <c r="T2">
-        <v>223.27183658974201</v>
+        <v>211.49503265162099</v>
       </c>
       <c r="U2">
-        <v>219.87444725693899</v>
+        <v>221.388463865094</v>
       </c>
       <c r="V2">
-        <v>220.25200205761701</v>
+        <v>235.225607808886</v>
       </c>
       <c r="W2">
-        <v>217.95717703185201</v>
+        <v>239.971586446266</v>
       </c>
       <c r="X2">
-        <v>273.00522467454999</v>
+        <v>340.37994583711099</v>
       </c>
       <c r="Y2">
-        <v>347.13972308848201</v>
+        <v>457.58083398530403</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -8740,7 +8740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Calculate MR for hours and weekdays
</commit_message>
<xml_diff>
--- a/document/temporal.xlsx
+++ b/document/temporal.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t>GR</t>
   </si>
@@ -1899,7 +1899,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.0586482730994081E-2"/>
+          <c:y val="5.4726368159203981E-2"/>
+          <c:w val="0.88609608218686498"/>
+          <c:h val="0.73990833235397813"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -2366,6 +2376,69 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Days of week</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.89890214438616478"/>
+              <c:y val="0.89014847024718924"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2431,6 +2504,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Waiting</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> time (seconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2544,6 +2678,716 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.2278435767415656E-2"/>
+          <c:y val="5.6628056628056631E-2"/>
+          <c:w val="0.89449644466145606"/>
+          <c:h val="0.72572239280900708"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>weekday!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ER Optimal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>weekday!$B$9:$H$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Monday</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tuesday</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Wednesday</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Thursday</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Friday</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Saturday</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sunday</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>weekday!$B$10:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>17.0607180401541</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.796139170293399</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.0912820643185</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.5856340998628</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.9509426479603</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34.233468327820198</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5665-48AD-9858-2131D6F15260}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>weekday!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>weekday!$B$9:$H$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Monday</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tuesday</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Wednesday</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Thursday</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Friday</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Saturday</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sunday</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>weekday!$B$11:$H$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>62.249449177868598</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>62.080827245567605</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>61.912059923113702</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>61.187719568836094</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>61.354384439270504</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64.467346586307499</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>61.654861374314997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5665-48AD-9858-2131D6F15260}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>weekday!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PR Optimal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>weekday!$B$9:$H$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Monday</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tuesday</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Wednesday</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Thursday</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Friday</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Saturday</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sunday</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>weekday!$B$12:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>7.4067821248508494</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.4675289013171806</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.2620174611183597</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.3867163341074695</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.4807921744960497</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.8786164335047</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.3384232920804</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5665-48AD-9858-2131D6F15260}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>weekday!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>weekday!$B$9:$H$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Monday</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tuesday</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Wednesday</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Thursday</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Friday</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Saturday</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sunday</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>weekday!$B$13:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.9809524081414702</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5871216191491202</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5273298975613501</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.2397847200951899</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.8925975692939798</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.5957981106828498</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.4742402521084301</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5665-48AD-9858-2131D6F15260}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2106594960"/>
+        <c:axId val="2106605360"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2106594960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Days</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of week</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.88490265815400371"/>
+              <c:y val="0.8708872201785588"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2106605360"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2106605360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Percentage</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (%)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2106594960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3869,7 +4713,1132 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.5046834196354181E-2"/>
+          <c:y val="5.0925925925925923E-2"/>
+          <c:w val="0.91517344142284884"/>
+          <c:h val="0.75797025371828508"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>hour!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ER Optimal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>hour!$B$10:$Y$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>hour!$B$11:$Y$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.8842249312275703</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.061129105889</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.3003484483707</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14.017313106694099</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.543577272417499</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.298285161787899</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14.4344273996068</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14.800405672768299</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.661641851194299</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.693430585566599</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14.476029495996501</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14.515900247273199</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15.200551005624799</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14.7639285591383</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>14.643130022394901</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14.250449955004498</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>14.9236805002145</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>14.5253195119595</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>14.031683589389099</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-73C3-429F-9869-B9E93BFBE76E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>hour!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>hour!$B$10:$Y$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>hour!$B$12:$Y$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3800781042922001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44.486831020615703</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>61.864767189213801</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>63.593661513382408</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>63.839915245432898</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>63.641756813577402</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>62.386698600935595</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>61.933995471845506</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>61.796121489413004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>62.168240692147606</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60.723097413430906</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>60.779681280015197</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>60.1884855437265</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>60.059592038153895</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>62.669413032163405</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>63.817138447664398</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>64.146228884600404</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>64.495895158796301</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>65.68755404521049</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>69.192362251754503</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-73C3-429F-9869-B9E93BFBE76E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>hour!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>hour!$B$10:$Y$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>hour!$B$13:$Y$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.197072072072072</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.69853045009084602</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.35885159080256</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5769569329140301</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.3999313733741596</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.5664288038501897</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.4329294819229297</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.37117396358</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.5265632675977203</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.7376534983525098</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.1314844664581498</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.4890554566431806</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.8816051770746407</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.9156992184536001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.94297440818523</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.1035195746517896</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.3931030810733995</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.9353123913555401</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.6332082893251196</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.2187586974672899</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-73C3-429F-9869-B9E93BFBE76E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>hour!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PR Optimal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>hour!$B$10:$Y$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>hour!$B$14:$Y$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.11528179442075799</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.7386324767789905</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.4247211908210096</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.8019167091791202</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.1766170793263004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.2502294708362705</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.6864596141895696</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.0346155124577905</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.1072507969532506</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.7098504798626504</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.7060665007786699</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.8793461783916801</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.4067149106687804</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.6960571040527999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.0601026795316901</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.6628189490177405</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.7574273896252297</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8.4242702246635801</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.2053753376039609</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.3411441152858696</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-73C3-429F-9869-B9E93BFBE76E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="90599664"/>
+        <c:axId val="90586352"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="90599664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Hour</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.94306950739566298"/>
+              <c:y val="0.90703630796150481"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="90586352"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="90586352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Percentage (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="90599664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4288,7 +6257,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4639,6 +6607,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -6149,7 +8197,7 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -6257,11 +8305,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -6272,11 +8315,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -6308,9 +8346,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6665,6 +8700,1038 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7249,16 +10316,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7277,6 +10344,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>300036</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7284,16 +10381,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7307,6 +10404,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>595312</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7618,7 +10745,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8014,10 +11141,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8175,6 +11302,130 @@
         <v>490.26873764211501</v>
       </c>
     </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>17.0607180401541</v>
+      </c>
+      <c r="C10">
+        <v>14.796139170293399</v>
+      </c>
+      <c r="D10">
+        <v>14.0912820643185</v>
+      </c>
+      <c r="E10">
+        <v>12.5856340998628</v>
+      </c>
+      <c r="F10">
+        <v>10.9509426479603</v>
+      </c>
+      <c r="H10">
+        <v>34.233468327820198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>62.249449177868598</v>
+      </c>
+      <c r="C11">
+        <v>62.080827245567605</v>
+      </c>
+      <c r="D11">
+        <v>61.912059923113702</v>
+      </c>
+      <c r="E11">
+        <v>61.187719568836094</v>
+      </c>
+      <c r="F11">
+        <v>61.354384439270504</v>
+      </c>
+      <c r="G11">
+        <v>64.467346586307499</v>
+      </c>
+      <c r="H11">
+        <v>61.654861374314997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>7.4067821248508494</v>
+      </c>
+      <c r="C12">
+        <v>7.4675289013171806</v>
+      </c>
+      <c r="D12">
+        <v>7.2620174611183597</v>
+      </c>
+      <c r="E12">
+        <v>7.3867163341074695</v>
+      </c>
+      <c r="F12">
+        <v>7.4807921744960497</v>
+      </c>
+      <c r="G12">
+        <v>11.8786164335047</v>
+      </c>
+      <c r="H12">
+        <v>10.3384232920804</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>3.9809524081414702</v>
+      </c>
+      <c r="C13">
+        <v>3.5871216191491202</v>
+      </c>
+      <c r="D13">
+        <v>3.5273298975613501</v>
+      </c>
+      <c r="E13">
+        <v>3.2397847200951899</v>
+      </c>
+      <c r="F13">
+        <v>2.8925975692939798</v>
+      </c>
+      <c r="G13">
+        <v>5.5957981106828498</v>
+      </c>
+      <c r="H13">
+        <v>3.4742402521084301</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8183,10 +11434,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y8"/>
+  <dimension ref="A1:Y14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="W39" sqref="W39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8728,6 +11979,388 @@
       </c>
       <c r="Y8">
         <v>883748</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>6</v>
+      </c>
+      <c r="H10">
+        <v>7</v>
+      </c>
+      <c r="I10">
+        <v>8</v>
+      </c>
+      <c r="J10">
+        <v>9</v>
+      </c>
+      <c r="K10">
+        <v>10</v>
+      </c>
+      <c r="L10">
+        <v>11</v>
+      </c>
+      <c r="M10">
+        <v>12</v>
+      </c>
+      <c r="N10">
+        <v>13</v>
+      </c>
+      <c r="O10">
+        <v>14</v>
+      </c>
+      <c r="P10">
+        <v>15</v>
+      </c>
+      <c r="Q10">
+        <v>16</v>
+      </c>
+      <c r="R10">
+        <v>17</v>
+      </c>
+      <c r="S10">
+        <v>18</v>
+      </c>
+      <c r="T10">
+        <v>19</v>
+      </c>
+      <c r="U10">
+        <v>20</v>
+      </c>
+      <c r="V10">
+        <v>21</v>
+      </c>
+      <c r="W10">
+        <v>22</v>
+      </c>
+      <c r="X10">
+        <v>23</v>
+      </c>
+      <c r="Y10">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>6.8842249312275703</v>
+      </c>
+      <c r="H11">
+        <v>13.061129105889</v>
+      </c>
+      <c r="I11">
+        <v>13.3003484483707</v>
+      </c>
+      <c r="J11">
+        <v>14.017313106694099</v>
+      </c>
+      <c r="K11">
+        <v>14.543577272417499</v>
+      </c>
+      <c r="L11">
+        <v>14.298285161787899</v>
+      </c>
+      <c r="M11">
+        <v>14.4344273996068</v>
+      </c>
+      <c r="N11">
+        <v>14.800405672768299</v>
+      </c>
+      <c r="O11">
+        <v>14.661641851194299</v>
+      </c>
+      <c r="P11">
+        <v>14.693430585566599</v>
+      </c>
+      <c r="Q11">
+        <v>14.476029495996501</v>
+      </c>
+      <c r="R11">
+        <v>14.515900247273199</v>
+      </c>
+      <c r="S11">
+        <v>15.200551005624799</v>
+      </c>
+      <c r="T11">
+        <v>14.7639285591383</v>
+      </c>
+      <c r="U11">
+        <v>14.643130022394901</v>
+      </c>
+      <c r="V11">
+        <v>14.250449955004498</v>
+      </c>
+      <c r="W11">
+        <v>14.9236805002145</v>
+      </c>
+      <c r="X11">
+        <v>14.5253195119595</v>
+      </c>
+      <c r="Y11">
+        <v>14.031683589389099</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>1.3800781042922001</v>
+      </c>
+      <c r="G12">
+        <v>44.486831020615703</v>
+      </c>
+      <c r="H12">
+        <v>61.864767189213801</v>
+      </c>
+      <c r="I12">
+        <v>63.593661513382408</v>
+      </c>
+      <c r="J12">
+        <v>63.839915245432898</v>
+      </c>
+      <c r="K12">
+        <v>63.641756813577402</v>
+      </c>
+      <c r="L12">
+        <v>62.386698600935595</v>
+      </c>
+      <c r="M12">
+        <v>61.933995471845506</v>
+      </c>
+      <c r="N12">
+        <v>61.796121489413004</v>
+      </c>
+      <c r="O12">
+        <v>62.168240692147606</v>
+      </c>
+      <c r="P12">
+        <v>60.723097413430906</v>
+      </c>
+      <c r="Q12">
+        <v>60.779681280015197</v>
+      </c>
+      <c r="R12">
+        <v>60.1884855437265</v>
+      </c>
+      <c r="S12">
+        <v>60.059592038153895</v>
+      </c>
+      <c r="T12">
+        <v>62.669413032163405</v>
+      </c>
+      <c r="U12">
+        <v>63.817138447664398</v>
+      </c>
+      <c r="V12">
+        <v>64.146228884600404</v>
+      </c>
+      <c r="W12">
+        <v>64.495895158796301</v>
+      </c>
+      <c r="X12">
+        <v>65.68755404521049</v>
+      </c>
+      <c r="Y12">
+        <v>69.192362251754503</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0.197072072072072</v>
+      </c>
+      <c r="G13">
+        <v>0.69853045009084602</v>
+      </c>
+      <c r="H13">
+        <v>1.35885159080256</v>
+      </c>
+      <c r="I13">
+        <v>2.5769569329140301</v>
+      </c>
+      <c r="J13">
+        <v>3.3999313733741596</v>
+      </c>
+      <c r="K13">
+        <v>3.5664288038501897</v>
+      </c>
+      <c r="L13">
+        <v>3.4329294819229297</v>
+      </c>
+      <c r="M13">
+        <v>3.37117396358</v>
+      </c>
+      <c r="N13">
+        <v>3.5265632675977203</v>
+      </c>
+      <c r="O13">
+        <v>3.7376534983525098</v>
+      </c>
+      <c r="P13">
+        <v>4.1314844664581498</v>
+      </c>
+      <c r="Q13">
+        <v>4.4890554566431806</v>
+      </c>
+      <c r="R13">
+        <v>4.8816051770746407</v>
+      </c>
+      <c r="S13">
+        <v>4.9156992184536001</v>
+      </c>
+      <c r="T13">
+        <v>4.94297440818523</v>
+      </c>
+      <c r="U13">
+        <v>4.1035195746517896</v>
+      </c>
+      <c r="V13">
+        <v>4.3931030810733995</v>
+      </c>
+      <c r="W13">
+        <v>3.9353123913555401</v>
+      </c>
+      <c r="X13">
+        <v>2.6332082893251196</v>
+      </c>
+      <c r="Y13">
+        <v>2.2187586974672899</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0.11528179442075799</v>
+      </c>
+      <c r="G14">
+        <v>4.7386324767789905</v>
+      </c>
+      <c r="H14">
+        <v>7.4247211908210096</v>
+      </c>
+      <c r="I14">
+        <v>7.8019167091791202</v>
+      </c>
+      <c r="J14">
+        <v>8.1766170793263004</v>
+      </c>
+      <c r="K14">
+        <v>8.2502294708362705</v>
+      </c>
+      <c r="L14">
+        <v>7.6864596141895696</v>
+      </c>
+      <c r="M14">
+        <v>8.0346155124577905</v>
+      </c>
+      <c r="N14">
+        <v>8.1072507969532506</v>
+      </c>
+      <c r="O14">
+        <v>8.7098504798626504</v>
+      </c>
+      <c r="P14">
+        <v>8.7060665007786699</v>
+      </c>
+      <c r="Q14">
+        <v>8.8793461783916801</v>
+      </c>
+      <c r="R14">
+        <v>8.4067149106687804</v>
+      </c>
+      <c r="S14">
+        <v>8.6960571040527999</v>
+      </c>
+      <c r="T14">
+        <v>9.0601026795316901</v>
+      </c>
+      <c r="U14">
+        <v>8.6628189490177405</v>
+      </c>
+      <c r="V14">
+        <v>8.7574273896252297</v>
+      </c>
+      <c r="W14">
+        <v>8.4242702246635801</v>
+      </c>
+      <c r="X14">
+        <v>9.2053753376039609</v>
+      </c>
+      <c r="Y14">
+        <v>9.3411441152858696</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update draft: modify conclusion and abstract
</commit_message>
<xml_diff>
--- a/document/temporal.xlsx
+++ b/document/temporal.xlsx
@@ -3418,8 +3418,593 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>hour!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ER Optimal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>hour!$B$1:$Y$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>hour!$B$6:$Y$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>84.975497261458599</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>226.72109875986101</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>245.20126294816399</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>214.66595700448099</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>245.31773626627501</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>280.28472677371701</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>284.32418415721799</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>287.22675744260698</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>315.39124460361597</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>319.68191515964099</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>299.707377441593</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>270.64001101906598</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>265.28042164473101</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>289.83414242946799</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>289.66494464008599</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>302.62426139415697</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>300.24863505043498</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>327.605941712478</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>485.05473015873002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>673.24427531436095</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-A2DD-49A6-B25C-8548F331CFE1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>hour!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>hour!$B$1:$Y$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>hour!$B$4:$Y$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>790</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>881.54750042143496</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>573.27544088084801</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>426.17247749285099</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>419.85933117117997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>483.03277848960698</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>499.31686221596402</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>501.79268138900699</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>506.379317575747</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>497.94991234365898</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>468.64238639489201</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>402.43289282212299</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>379.38027682813401</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>390.76085298941501</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>413.88287881732498</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>482.572612738494</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>562.923430075331</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>599.19591124192004</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1171.0598402942301</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1781.77392684148</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A2DD-49A6-B25C-8548F331CFE1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>hour!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>hour!$B$1:$Y$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>hour!$B$5:$Y$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>99.443427400116605</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>781.299124476369</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>715.19837329148299</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>532.13935203317396</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>524.20777871964196</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>593.51294216581903</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>605.68257893129896</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>607.36074861494103</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>610.54952332511004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>603.52653368445897</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>559.03767308288604</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>481.16624504045097</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>451.527003495082</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>471.88005197125301</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>508.93107841691301</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>604.77887010527104</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>702.22212758276601</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>761.96522117129405</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1469.8614438529701</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2470.2432645747499</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A2DD-49A6-B25C-8548F331CFE1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>hour!$A$2</c:f>
@@ -3614,7 +4199,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>hour!$A$3</c:f>
@@ -3804,591 +4389,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-A2DD-49A6-B25C-8548F331CFE1}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>hour!$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>AR</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>hour!$B$1:$Y$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>24</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>hour!$B$4:$Y$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>790</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>881.54750042143496</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>573.27544088084801</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>426.17247749285099</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>419.85933117117997</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>483.03277848960698</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>499.31686221596402</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>501.79268138900699</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>506.379317575747</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>497.94991234365898</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>468.64238639489201</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>402.43289282212299</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>379.38027682813401</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>390.76085298941501</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>413.88287881732498</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>482.572612738494</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>562.923430075331</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>599.19591124192004</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1171.0598402942301</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1781.77392684148</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-A2DD-49A6-B25C-8548F331CFE1}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>hour!$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>GR</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>hour!$B$1:$Y$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>24</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>hour!$B$5:$Y$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>99.443427400116605</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>781.299124476369</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>715.19837329148299</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>532.13935203317396</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>524.20777871964196</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>593.51294216581903</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>605.68257893129896</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>607.36074861494103</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>610.54952332511004</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>603.52653368445897</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>559.03767308288604</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>481.16624504045097</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>451.527003495082</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>471.88005197125301</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>508.93107841691301</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>604.77887010527104</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>702.22212758276601</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>761.96522117129405</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1469.8614438529701</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2470.2432645747499</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-A2DD-49A6-B25C-8548F331CFE1}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>hour!$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ER Optimal</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>hour!$B$1:$Y$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>24</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>hour!$B$6:$Y$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>84.975497261458599</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>226.72109875986101</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>245.20126294816399</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>214.66595700448099</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>245.31773626627501</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>280.28472677371701</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>284.32418415721799</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>287.22675744260698</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>315.39124460361597</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>319.68191515964099</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>299.707377441593</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>270.64001101906598</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>265.28042164473101</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>289.83414242946799</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>289.66494464008599</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>302.62426139415697</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>300.24863505043498</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>327.605941712478</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>485.05473015873002</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>673.24427531436095</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-A2DD-49A6-B25C-8548F331CFE1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4955,7 +4955,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -5134,8 +5134,203 @@
           </c:extLst>
         </c:ser>
         <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>hour!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PR Optimal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>hour!$B$10:$Y$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>hour!$B$14:$Y$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.11528179442075799</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.7386324767789905</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.4247211908210096</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.8019167091791202</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.1766170793263004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.2502294708362705</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.6864596141895696</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.0346155124577905</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.1072507969532506</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.7098504798626504</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.7060665007786699</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.8793461783916801</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.4067149106687804</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.6960571040527999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.0601026795316901</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.6628189490177405</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.7574273896252297</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8.4242702246635801</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.2053753376039609</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.3411441152858696</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-73C3-429F-9869-B9E93BFBE76E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>hour!$A$13</c:f>
@@ -5325,201 +5520,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-73C3-429F-9869-B9E93BFBE76E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>hour!$A$14</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>PR Optimal</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>hour!$B$10:$Y$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>24</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>hour!$B$14:$Y$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.11528179442075799</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.7386324767789905</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.4247211908210096</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.8019167091791202</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8.1766170793263004</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>8.2502294708362705</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7.6864596141895696</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>8.0346155124577905</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>8.1072507969532506</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8.7098504798626504</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>8.7060665007786699</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>8.8793461783916801</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>8.4067149106687804</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>8.6960571040527999</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>9.0601026795316901</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>8.6628189490177405</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>8.7574273896252297</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>8.4242702246635801</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>9.2053753376039609</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>9.3411441152858696</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-73C3-429F-9869-B9E93BFBE76E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -11143,7 +11143,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
@@ -11436,8 +11436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="W39" sqref="W39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>